<commit_message>
Cleaned up run_powerflow.py, reformatted hunting_results.xlsx to remove unecessary columns and resize properly
</commit_message>
<xml_diff>
--- a/hunting_results.xlsx
+++ b/hunting_results.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birkaransachdev/Desktop/Research/openDSSstarterCodeSharedNew/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563EB2D7-B2BF-3249-9644-48EA47CF715F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>timestamp of run</t>
   </si>
@@ -28,24 +22,15 @@
     <t>feeder_name</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>high_node</t>
   </si>
   <si>
     <t>low_node</t>
   </si>
   <si>
-    <t>high_V</t>
-  </si>
-  <si>
-    <t>low_V</t>
-  </si>
-  <si>
-    <t>high_V (p.u.)</t>
-  </si>
-  <si>
-    <t>low_V (p.u.)</t>
-  </si>
-  <si>
     <t>num_high_nodes</t>
   </si>
   <si>
@@ -67,26 +52,29 @@
     <t>index</t>
   </si>
   <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Overvoltage</t>
+  </si>
+  <si>
+    <t>Undervoltage</t>
+  </si>
+  <si>
     <t>Bus_48</t>
   </si>
   <si>
-    <t>Bus_151</t>
-  </si>
-  <si>
     <t>Bus_83</t>
-  </si>
-  <si>
-    <t>Bus_79</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,14 +138,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -204,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,27 +216,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,24 +250,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,18 +425,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -527,296 +483,157 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>44510.846020335652</v>
+        <v>44515.82595831018</v>
       </c>
       <c r="C2">
         <v>123</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>1.1000000000000001</v>
+      <c r="F2" t="s">
+        <v>16</v>
       </c>
       <c r="G2">
-        <v>0.60000000000000009</v>
+        <v>8</v>
       </c>
       <c r="H2">
-        <v>1.084887879063821</v>
+        <v>-610.5593010432244</v>
       </c>
       <c r="I2">
-        <v>0.93348028994072407</v>
+        <v>-295.5107017049206</v>
       </c>
       <c r="J2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K2">
-        <v>-1448.7847821364651</v>
+        <v>166.6756712617998</v>
       </c>
       <c r="L2">
-        <v>-701.21183455404901</v>
-      </c>
-      <c r="M2">
-        <v>16</v>
-      </c>
-      <c r="N2">
-        <v>707.89484178924545</v>
-      </c>
-      <c r="O2">
-        <v>342.62110342599482</v>
+        <v>80.6710248907111</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>44510.847919293978</v>
+        <v>44515.82981092593</v>
       </c>
       <c r="C3">
         <v>123</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3">
-        <v>1.4</v>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
       <c r="G3">
-        <v>0.9</v>
+        <v>8</v>
       </c>
       <c r="H3">
-        <v>1.192973545729918</v>
+        <v>-610.5593010432244</v>
       </c>
       <c r="I3">
-        <v>1.083519966792456</v>
+        <v>-295.5107017049206</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K3">
-        <v>-6623.0161469095601</v>
+        <v>561.4338400397465</v>
       </c>
       <c r="L3">
-        <v>-3205.5398151042268</v>
-      </c>
-      <c r="M3">
-        <v>16</v>
-      </c>
-      <c r="N3">
-        <v>210.1562811561823</v>
-      </c>
-      <c r="O3">
-        <v>101.71564007959221</v>
+        <v>271.7339785792373</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>44510.851127916663</v>
+        <v>44515.83511534722</v>
       </c>
       <c r="C4">
         <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>1.5</v>
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
       </c>
       <c r="G4">
-        <v>0.9</v>
+        <v>8</v>
       </c>
       <c r="H4">
-        <v>1.140948249265801</v>
+        <v>-610.5593010432244</v>
       </c>
       <c r="I4">
-        <v>1.0611617855143749</v>
+        <v>-295.5107017049206</v>
       </c>
       <c r="J4">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K4">
-        <v>-3592.581942001912</v>
+        <v>166.6756712617998</v>
       </c>
       <c r="L4">
-        <v>-1738.8096599289261</v>
-      </c>
-      <c r="M4">
-        <v>16</v>
-      </c>
-      <c r="N4">
-        <v>210.1562811561823</v>
-      </c>
-      <c r="O4">
-        <v>101.71564007959221</v>
+        <v>80.6710248907111</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>44510.854681666657</v>
-      </c>
-      <c r="C5">
-        <v>123</v>
+        <v>44515.83553325033</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5">
-        <v>1.1000000000000001</v>
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
       </c>
       <c r="G5">
-        <v>0.50000000000000011</v>
+        <v>8</v>
       </c>
       <c r="H5">
-        <v>1.003371792522729</v>
+        <v>-610.5593010432244</v>
       </c>
       <c r="I5">
-        <v>0.92705326435496171</v>
+        <v>-295.5107017049206</v>
       </c>
       <c r="J5">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K5">
-        <v>-603.55376625632061</v>
+        <v>166.6756712617998</v>
       </c>
       <c r="L5">
-        <v>-292.12002286805921</v>
-      </c>
-      <c r="M5">
-        <v>16</v>
-      </c>
-      <c r="N5">
-        <v>829.56426772177235</v>
-      </c>
-      <c r="O5">
-        <v>401.50910557733778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>44510.858132777779</v>
-      </c>
-      <c r="C6">
-        <v>123</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6">
-        <v>1.4</v>
-      </c>
-      <c r="G6">
-        <v>0.9</v>
-      </c>
-      <c r="H6">
-        <v>1.0816513238370269</v>
-      </c>
-      <c r="I6">
-        <v>1.0046479635587411</v>
-      </c>
-      <c r="J6">
-        <v>11</v>
-      </c>
-      <c r="K6">
-        <v>-2759.102931457468</v>
-      </c>
-      <c r="L6">
-        <v>-1335.4058188254151</v>
-      </c>
-      <c r="M6">
-        <v>13</v>
-      </c>
-      <c r="N6">
-        <v>352.53566479988638</v>
-      </c>
-      <c r="O6">
-        <v>170.62726176314499</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>44510.859492708332</v>
-      </c>
-      <c r="C7">
-        <v>123</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G7">
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="H7">
-        <v>0.98077902823052632</v>
-      </c>
-      <c r="I7">
-        <v>0.90157897828056244</v>
-      </c>
-      <c r="J7">
-        <v>11</v>
-      </c>
-      <c r="K7">
-        <v>-603.55376625632061</v>
-      </c>
-      <c r="L7">
-        <v>-292.12002286805921</v>
-      </c>
-      <c r="M7">
-        <v>13</v>
-      </c>
-      <c r="N7">
-        <v>1187.4885551154071</v>
-      </c>
-      <c r="O7">
-        <v>574.74446067585677</v>
+        <v>80.6710248907111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated hunting_results.xlsx to include more sample runs
</commit_message>
<xml_diff>
--- a/hunting_results.xlsx
+++ b/hunting_results.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birkaransachdev/Desktop/Research/openDSSstarterCodeSharedNew/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA15A378-74B3-6049-87C2-EA1ED4CBAFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="20860" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>timestamp of run</t>
   </si>
@@ -52,9 +58,6 @@
     <t>index</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
     <t>Overvoltage</t>
   </si>
   <si>
@@ -64,17 +67,23 @@
     <t>Bus_48</t>
   </si>
   <si>
+    <t>Bus_151</t>
+  </si>
+  <si>
     <t>Bus_83</t>
+  </si>
+  <si>
+    <t>Bus_79</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +147,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -184,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,9 +233,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,6 +285,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,28 +478,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -484,21 +538,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>44515.82595831018</v>
+        <v>44515.825958310183</v>
       </c>
       <c r="C2">
         <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -507,36 +561,36 @@
         <v>8</v>
       </c>
       <c r="H2">
-        <v>-610.5593010432244</v>
+        <v>-610.55930104322442</v>
       </c>
       <c r="I2">
-        <v>-295.5107017049206</v>
+        <v>-295.51070170492062</v>
       </c>
       <c r="J2">
         <v>16</v>
       </c>
       <c r="K2">
-        <v>166.6756712617998</v>
+        <v>166.67567126179981</v>
       </c>
       <c r="L2">
-        <v>80.6710248907111</v>
+        <v>80.671024890711095</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>44515.82981092593</v>
+        <v>44515.829810925927</v>
       </c>
       <c r="C3">
         <v>123</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -545,33 +599,33 @@
         <v>8</v>
       </c>
       <c r="H3">
-        <v>-610.5593010432244</v>
+        <v>-610.55930104322442</v>
       </c>
       <c r="I3">
-        <v>-295.5107017049206</v>
+        <v>-295.51070170492062</v>
       </c>
       <c r="J3">
         <v>16</v>
       </c>
       <c r="K3">
-        <v>561.4338400397465</v>
+        <v>561.43384003974654</v>
       </c>
       <c r="L3">
-        <v>271.7339785792373</v>
+        <v>271.73397857923732</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>44515.83511534722</v>
+        <v>44519.68430940972</v>
       </c>
       <c r="C4">
         <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -580,33 +634,33 @@
         <v>16</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H4">
-        <v>-610.5593010432244</v>
+        <v>-707.89484178924647</v>
       </c>
       <c r="I4">
-        <v>-295.5107017049206</v>
+        <v>-342.62110342599527</v>
       </c>
       <c r="J4">
         <v>16</v>
       </c>
       <c r="K4">
-        <v>166.6756712617998</v>
+        <v>166.67567126179981</v>
       </c>
       <c r="L4">
-        <v>80.6710248907111</v>
+        <v>80.671024890711095</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>44515.83553325033</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>44519.690525034719</v>
+      </c>
+      <c r="C5">
+        <v>123</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -618,22 +672,174 @@
         <v>16</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H5">
-        <v>-610.5593010432244</v>
+        <v>-707.89484178924567</v>
       </c>
       <c r="I5">
-        <v>-295.5107017049206</v>
+        <v>-342.62110342599487</v>
       </c>
       <c r="J5">
         <v>16</v>
       </c>
       <c r="K5">
-        <v>166.6756712617998</v>
+        <v>657.93028129657807</v>
       </c>
       <c r="L5">
-        <v>80.6710248907111</v>
+        <v>318.43825614754383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44519.687113819447</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>-707.89484178924647</v>
+      </c>
+      <c r="I6">
+        <v>-342.62110342599527</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+      <c r="K6">
+        <v>260.0672937048343</v>
+      </c>
+      <c r="L6">
+        <v>125.8725701531398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44519.688869687503</v>
+      </c>
+      <c r="C7">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>-707.89484178924567</v>
+      </c>
+      <c r="I7">
+        <v>-342.62110342599487</v>
+      </c>
+      <c r="J7">
+        <v>13</v>
+      </c>
+      <c r="K7">
+        <v>698.07536731297603</v>
+      </c>
+      <c r="L7">
+        <v>337.86847777948037</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44519.691084571758</v>
+      </c>
+      <c r="C8">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>-1279.2671069477101</v>
+      </c>
+      <c r="I8">
+        <v>-619.16527976269151</v>
+      </c>
+      <c r="J8">
+        <v>13</v>
+      </c>
+      <c r="K8">
+        <v>260.0672937048343</v>
+      </c>
+      <c r="L8">
+        <v>125.8725701531398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44519.692170556627</v>
+      </c>
+      <c r="C9">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>-1279.267106947708</v>
+      </c>
+      <c r="I9">
+        <v>-619.16527976269072</v>
+      </c>
+      <c r="J9">
+        <v>13</v>
+      </c>
+      <c r="K9">
+        <v>876.0161472162838</v>
+      </c>
+      <c r="L9">
+        <v>423.99181525268131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited hunting_results.xlsx to include the actual hi and lo node voltage values
</commit_message>
<xml_diff>
--- a/hunting_results.xlsx
+++ b/hunting_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birkaransachdev/Desktop/Research/openDSSstarterCodeSharedNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA15A378-74B3-6049-87C2-EA1ED4CBAFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784937E0-C27E-A24F-B0D0-FEBFFD33A9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="20860" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>timestamp of run</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Q_per_lo (kVAR)</t>
+  </si>
+  <si>
+    <t>V_hi (V p.u.)</t>
+  </si>
+  <si>
+    <t>V_lo (V p.u.)</t>
   </si>
   <si>
     <t>index</t>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -498,11 +504,12 @@
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="11" width="13.6640625" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="14" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -537,34 +544,40 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>44515.825958310183</v>
+        <v>44560.713970717603</v>
       </c>
       <c r="C2">
         <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>8</v>
       </c>
       <c r="H2">
-        <v>-610.55930104322442</v>
+        <v>-1279.2671069477101</v>
       </c>
       <c r="I2">
-        <v>-295.51070170492062</v>
+        <v>-619.16527976269151</v>
       </c>
       <c r="J2">
         <v>16</v>
@@ -575,63 +588,75 @@
       <c r="L2">
         <v>80.671024890711095</v>
       </c>
+      <c r="M2">
+        <v>1.1618999999999999</v>
+      </c>
+      <c r="N2">
+        <v>1.0115000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>44515.829810925927</v>
+        <v>44560.716146851853</v>
       </c>
       <c r="C3">
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G3">
         <v>8</v>
       </c>
       <c r="H3">
-        <v>-610.55930104322442</v>
+        <v>-1279.267106947708</v>
       </c>
       <c r="I3">
-        <v>-295.51070170492062</v>
+        <v>-619.16527976269072</v>
       </c>
       <c r="J3">
         <v>16</v>
       </c>
       <c r="K3">
-        <v>561.43384003974654</v>
+        <v>736.88191505216741</v>
       </c>
       <c r="L3">
-        <v>271.73397857923732</v>
+        <v>356.650846885249</v>
+      </c>
+      <c r="M3">
+        <v>1.0765</v>
+      </c>
+      <c r="N3">
+        <v>0.94199999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>44519.68430940972</v>
+        <v>44560.716822361108</v>
       </c>
       <c r="C4">
         <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G4">
         <v>11</v>
@@ -651,25 +676,31 @@
       <c r="L4">
         <v>80.671024890711095</v>
       </c>
+      <c r="M4">
+        <v>1.0936999999999999</v>
+      </c>
+      <c r="N4">
+        <v>0.99909999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>44519.690525034719</v>
+        <v>44560.718002013891</v>
       </c>
       <c r="C5">
         <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>11</v>
@@ -689,25 +720,31 @@
       <c r="L5">
         <v>318.43825614754383</v>
       </c>
+      <c r="M5">
+        <v>1.0431999999999999</v>
+      </c>
+      <c r="N5">
+        <v>0.94410000000000005</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>44519.687113819447</v>
+        <v>44560.71876945602</v>
       </c>
       <c r="C6">
         <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <v>11</v>
@@ -727,25 +764,31 @@
       <c r="L6">
         <v>125.8725701531398</v>
       </c>
+      <c r="M6">
+        <v>1.0833999999999999</v>
+      </c>
+      <c r="N6">
+        <v>0.9879</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>44519.688869687503</v>
+        <v>44560.719873564813</v>
       </c>
       <c r="C7">
         <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>11</v>
@@ -765,25 +808,31 @@
       <c r="L7">
         <v>337.86847777948037</v>
       </c>
+      <c r="M7">
+        <v>1.044</v>
+      </c>
+      <c r="N7">
+        <v>0.94520000000000004</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>44519.691084571758</v>
+        <v>44560.720654606477</v>
       </c>
       <c r="C8">
         <v>123</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8">
         <v>8</v>
@@ -803,25 +852,31 @@
       <c r="L8">
         <v>125.8725701531398</v>
       </c>
+      <c r="M8">
+        <v>1.1395</v>
+      </c>
+      <c r="N8">
+        <v>0.99850000000000005</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>44519.692170556627</v>
+        <v>44560.721680410657</v>
       </c>
       <c r="C9">
         <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -840,6 +895,12 @@
       </c>
       <c r="L9">
         <v>423.99181525268131</v>
+      </c>
+      <c r="M9">
+        <v>1.071</v>
+      </c>
+      <c r="N9">
+        <v>0.93779999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>